<commit_message>
adding selling and buying costs
</commit_message>
<xml_diff>
--- a/cea/databases/SG/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/SG/lifecycle/LCA_infrastructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhargava\Documents\GitHub\CityEnergyAnalyst\cea\databases\SIN\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2870" windowWidth="28800" windowHeight="16260" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2865" windowWidth="28800" windowHeight="16260" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -104,12 +104,26 @@
         </r>
       </text>
     </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Selling price in US$(2015)/kWh(resource [thermal in case of fuels]).yr</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="53">
   <si>
     <t>Description</t>
   </si>
@@ -265,6 +279,9 @@
   </si>
   <si>
     <t>PEN and CO2 zero equivalent due to renewable technology, cost from CEA, costs in USD-2015</t>
+  </si>
+  <si>
+    <t>costs_sell_kWh</t>
   </si>
 </sst>
 </file>
@@ -738,17 +755,17 @@
       <selection activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.26953125" customWidth="1"/>
-    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -768,7 +785,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -788,7 +805,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -808,7 +825,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -843,17 +860,17 @@
       <selection activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -873,7 +890,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -893,7 +910,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
@@ -913,7 +930,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -947,17 +964,17 @@
       <selection activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="2" width="7.26953125" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -977,7 +994,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -997,7 +1014,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1017,7 +1034,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1037,7 +1054,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1057,7 +1074,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1077,7 +1094,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
@@ -1111,15 +1128,15 @@
       <selection activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1139,7 +1156,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1159,7 +1176,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1179,7 +1196,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -1206,20 +1223,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" customWidth="1"/>
-    <col min="6" max="6" width="123" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="123" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1235,11 +1253,14 @@
       <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1255,9 +1276,12 @@
       <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -1275,11 +1299,15 @@
         <f>4.94/293</f>
         <v>1.6860068259385668E-2</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="2">
+        <f>4.94/293</f>
+        <v>1.6860068259385668E-2</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1296,11 +1324,15 @@
         <f>0.2*0.75</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="2">
+        <f>0.2*0.75</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1316,7 +1348,10 @@
       <c r="E5" s="2">
         <v>1E-4</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>